<commit_message>
uploading data needed for figure 5&6
</commit_message>
<xml_diff>
--- a/Data/sgRNA/Figure5/N100M_sequence_result/N100M_plot.xlsx
+++ b/Data/sgRNA/Figure5/N100M_sequence_result/N100M_plot.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="47">
   <si>
     <t>base_name</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>(AAU)</t>
+  </si>
+  <si>
+    <t>Intact</t>
   </si>
   <si>
     <t>native 3'</t>
@@ -174,13 +177,15 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
-  <numFmts count="4">
+  <numFmts count="6">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="0.000"/>
+    <numFmt numFmtId="179" formatCode="#0.####"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -198,13 +203,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -354,7 +352,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -565,12 +563,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="9">
     <border>
@@ -681,28 +673,31 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -711,122 +706,119 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -835,8 +827,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -1188,8 +1188,8 @@
   <sheetPr/>
   <dimension ref="A1:AC187"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="E56" sqref="E56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
@@ -1393,16 +1393,16 @@
       <c r="AC8" s="5"/>
     </row>
     <row r="9" spans="1:29">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="6">
         <v>3564.57032432831</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="6">
         <v>4443165.56</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="6">
         <v>6.65801034328143</v>
       </c>
       <c r="E9" t="str">
@@ -2941,9 +2941,6 @@
       <c r="A82" t="s">
         <v>15</v>
       </c>
-      <c r="B82"/>
-      <c r="C82"/>
-      <c r="D82"/>
       <c r="E82" t="s">
         <v>14</v>
       </c>
@@ -2986,7 +2983,7 @@
         <v>7.47073565281232</v>
       </c>
       <c r="E84" t="str">
-        <f t="shared" ref="E84:E115" si="3">E83</f>
+        <f t="shared" ref="E84:E118" si="3">E83</f>
         <v>5'</v>
       </c>
       <c r="F84">
@@ -3658,7 +3655,7 @@
         <v>15.0869539594332</v>
       </c>
       <c r="E116" t="str">
-        <f>E115</f>
+        <f t="shared" si="3"/>
         <v>5'</v>
       </c>
       <c r="F116">
@@ -3679,7 +3676,7 @@
         <v>15.1231340523243</v>
       </c>
       <c r="E117" t="str">
-        <f>E116</f>
+        <f t="shared" si="3"/>
         <v>5'</v>
       </c>
       <c r="F117">
@@ -3700,7 +3697,7 @@
         <v>15.2090786671321</v>
       </c>
       <c r="E118" t="str">
-        <f>E117</f>
+        <f t="shared" si="3"/>
         <v>5'</v>
       </c>
       <c r="F118">
@@ -3976,65 +3973,125 @@
         <v>60</v>
       </c>
     </row>
+    <row r="133" spans="1:6">
+      <c r="A133" t="s">
+        <v>9</v>
+      </c>
+      <c r="B133" s="7">
+        <v>32099.2811157233</v>
+      </c>
+      <c r="C133" s="8">
+        <v>427089.01</v>
+      </c>
+      <c r="D133" s="9">
+        <v>17.5162381008943</v>
+      </c>
+      <c r="E133" t="s">
+        <v>17</v>
+      </c>
+      <c r="F133">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6">
+      <c r="A134" t="s">
+        <v>9</v>
+      </c>
+      <c r="B134" s="7">
+        <v>32099.2811157233</v>
+      </c>
+      <c r="C134" s="8">
+        <v>427089.01</v>
+      </c>
+      <c r="D134" s="9">
+        <v>17.5162381008943</v>
+      </c>
+      <c r="E134" t="s">
+        <v>14</v>
+      </c>
+      <c r="F134">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6">
+      <c r="A135" t="s">
+        <v>9</v>
+      </c>
+      <c r="B135" s="7">
+        <v>32099.2811157233</v>
+      </c>
+      <c r="C135" s="8">
+        <v>427089.01</v>
+      </c>
+      <c r="D135" s="9">
+        <v>17.5162381008943</v>
+      </c>
+      <c r="E135" t="s">
+        <v>7</v>
+      </c>
+      <c r="F135">
+        <v>100</v>
+      </c>
+    </row>
     <row r="167" spans="5:6">
-      <c r="E167" s="8"/>
-      <c r="F167" s="8"/>
+      <c r="E167" s="10"/>
+      <c r="F167" s="10"/>
     </row>
     <row r="168" spans="5:6">
-      <c r="E168" s="8"/>
-      <c r="F168" s="8"/>
+      <c r="E168" s="10"/>
+      <c r="F168" s="10"/>
     </row>
     <row r="169" spans="5:6">
-      <c r="E169" s="8"/>
-      <c r="F169" s="8"/>
+      <c r="E169" s="10"/>
+      <c r="F169" s="10"/>
     </row>
     <row r="170" spans="5:6">
-      <c r="E170" s="8"/>
-      <c r="F170" s="8"/>
+      <c r="E170" s="10"/>
+      <c r="F170" s="10"/>
     </row>
     <row r="171" spans="5:6">
-      <c r="E171" s="8"/>
-      <c r="F171" s="8"/>
+      <c r="E171" s="10"/>
+      <c r="F171" s="10"/>
     </row>
     <row r="172" spans="5:6">
-      <c r="E172" s="8"/>
-      <c r="F172" s="8"/>
+      <c r="E172" s="10"/>
+      <c r="F172" s="10"/>
     </row>
     <row r="173" spans="5:6">
-      <c r="E173" s="8"/>
-      <c r="F173" s="8"/>
+      <c r="E173" s="10"/>
+      <c r="F173" s="10"/>
     </row>
     <row r="174" spans="5:6">
-      <c r="E174" s="8"/>
-      <c r="F174" s="8"/>
+      <c r="E174" s="10"/>
+      <c r="F174" s="10"/>
     </row>
     <row r="181" spans="5:6">
-      <c r="E181" s="8"/>
-      <c r="F181" s="8"/>
+      <c r="E181" s="10"/>
+      <c r="F181" s="10"/>
     </row>
     <row r="182" spans="5:6">
-      <c r="E182" s="8"/>
-      <c r="F182" s="8"/>
+      <c r="E182" s="10"/>
+      <c r="F182" s="10"/>
     </row>
     <row r="183" spans="5:6">
-      <c r="E183" s="8"/>
-      <c r="F183" s="8"/>
+      <c r="E183" s="10"/>
+      <c r="F183" s="10"/>
     </row>
     <row r="184" spans="5:6">
-      <c r="E184" s="8"/>
-      <c r="F184" s="8"/>
+      <c r="E184" s="10"/>
+      <c r="F184" s="10"/>
     </row>
     <row r="185" spans="5:6">
-      <c r="E185" s="8"/>
-      <c r="F185" s="8"/>
+      <c r="E185" s="10"/>
+      <c r="F185" s="10"/>
     </row>
     <row r="186" spans="5:6">
-      <c r="E186" s="8"/>
-      <c r="F186" s="8"/>
+      <c r="E186" s="10"/>
+      <c r="F186" s="10"/>
     </row>
     <row r="187" spans="5:6">
-      <c r="E187" s="8"/>
-      <c r="F187" s="8"/>
+      <c r="E187" s="10"/>
+      <c r="F187" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4060,43 +4117,43 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="M1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
       <c r="S1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="U1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="19:19">
       <c r="S2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="12:16">
@@ -4105,7 +4162,7 @@
         <v>1292.2316559679</v>
       </c>
       <c r="M4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="N4">
         <v>1292.2316559679</v>
@@ -4153,7 +4210,7 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B6">
         <v>1904.34264690731</v>
@@ -4346,9 +4403,8 @@
       <c r="D11">
         <v>6.65801034328143</v>
       </c>
-      <c r="E11"/>
       <c r="F11">
-        <f>H11-B11</f>
+        <f t="shared" si="1"/>
         <v>21.9802978395301</v>
       </c>
       <c r="G11" t="s">
@@ -4490,7 +4546,7 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B16">
         <v>5179.77434890957</v>
@@ -4506,7 +4562,7 @@
         <v>21.9793644332503</v>
       </c>
       <c r="G16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H16">
         <v>5201.75371334282</v>
@@ -5324,7 +5380,7 @@
         <v>16.136828825442</v>
       </c>
       <c r="G53" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H53">
         <v>16995.2091105164</v>
@@ -5474,7 +5530,7 @@
     </row>
     <row r="62" spans="19:22">
       <c r="S62" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="T62">
         <v>19893.7135578117</v>
@@ -5724,58 +5780,58 @@
   <sheetData>
     <row r="1" spans="1:31">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D1" s="1"/>
       <c r="H1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="M1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="O1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="T1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="Z1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AA1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AD1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AE1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:30">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="S2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Z2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AD2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="7:11">
@@ -5828,7 +5884,7 @@
         <v>1856.22742503156</v>
       </c>
       <c r="H6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I6" s="3">
         <v>1856.22742503156</v>
@@ -5844,7 +5900,7 @@
         <v>18.01105863209</v>
       </c>
       <c r="S6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="T6">
         <v>1874.23848366365</v>
@@ -5859,7 +5915,7 @@
         <v>16</v>
       </c>
       <c r="X6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:24">
@@ -5903,7 +5959,7 @@
         <v>16</v>
       </c>
       <c r="X7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:24">
@@ -5947,7 +6003,7 @@
         <v>16</v>
       </c>
       <c r="X8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:24">
@@ -5991,7 +6047,7 @@
         <v>16</v>
       </c>
       <c r="X9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:24">
@@ -6035,7 +6091,7 @@
         <v>16</v>
       </c>
       <c r="X10" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:24">
@@ -6052,7 +6108,7 @@
         <v>6.3599807436943</v>
       </c>
       <c r="G11">
-        <f>I11-B11</f>
+        <f t="shared" si="0"/>
         <v>-8.01471902250023</v>
       </c>
       <c r="H11" t="s">
@@ -6087,7 +6143,7 @@
         <v>16</v>
       </c>
       <c r="X11" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:24">
@@ -6139,7 +6195,7 @@
         <v>16</v>
       </c>
       <c r="X12" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:24">
@@ -6172,7 +6228,7 @@
         <v>7.290118318367</v>
       </c>
       <c r="R13">
-        <f>T13-I13</f>
+        <f t="shared" si="2"/>
         <v>18.0119049783098</v>
       </c>
       <c r="S13" s="4" t="s">
@@ -6191,7 +6247,7 @@
         <v>16</v>
       </c>
       <c r="X13" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -6466,7 +6522,7 @@
     </row>
     <row r="23" spans="1:11">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B23">
         <v>7372.98369925016</v>
@@ -6556,7 +6612,7 @@
         <v>-18.0092189267198</v>
       </c>
       <c r="N26" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O26">
         <v>8335.1011393888</v>
@@ -6940,7 +6996,7 @@
         <v>14142.8871309032</v>
       </c>
       <c r="AD44" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AE44">
         <v>14142.8871309032</v>
@@ -7094,7 +7150,7 @@
     </row>
     <row r="53" spans="1:29">
       <c r="A53" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B53">
         <v>16995.2091105164</v>
@@ -7106,7 +7162,7 @@
         <v>15.7203694855849</v>
       </c>
       <c r="Z53" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AA53">
         <v>16995.2091105164</v>
@@ -7184,10 +7240,10 @@
         <v>15.960269118913</v>
       </c>
       <c r="E57" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F57" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="58" spans="1:4">

</xml_diff>

<commit_message>
small changes on the df
</commit_message>
<xml_diff>
--- a/Data/sgRNA/Figure5/N100M_sequence_result/N100M_plot.xlsx
+++ b/Data/sgRNA/Figure5/N100M_sequence_result/N100M_plot.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="17160"/>
+    <workbookView windowHeight="14460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="47">
   <si>
     <t>base_name</t>
   </si>
@@ -1189,7 +1189,7 @@
   <dimension ref="A1:AC187"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F135"/>
+      <selection activeCell="F132" sqref="A126:F132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
@@ -1200,6 +1200,8 @@
     <col min="4" max="4" width="12.6875" customWidth="1"/>
     <col min="5" max="5" width="11.375" customWidth="1"/>
     <col min="6" max="6" width="12.6875"/>
+    <col min="7" max="7" width="13.8125"/>
+    <col min="8" max="9" width="12.6875"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:6">
@@ -1277,7 +1279,7 @@
         <v>1.05053326047262</v>
       </c>
       <c r="E4" t="str">
-        <f t="shared" ref="E4:E35" si="0">E3</f>
+        <f>E3</f>
         <v>3'</v>
       </c>
       <c r="F4">
@@ -1298,12 +1300,13 @@
         <v>1.23111104326248</v>
       </c>
       <c r="E5" t="str">
-        <f t="shared" si="0"/>
+        <f>E4</f>
         <v>3'</v>
       </c>
       <c r="F5">
         <v>7</v>
       </c>
+      <c r="G5"/>
       <c r="T5" s="5"/>
       <c r="U5" s="5"/>
       <c r="V5" s="5"/>
@@ -1323,7 +1326,7 @@
         <v>1.89024456100464</v>
       </c>
       <c r="E6" t="str">
-        <f t="shared" si="0"/>
+        <f>E5</f>
         <v>3'</v>
       </c>
       <c r="F6">
@@ -1348,12 +1351,13 @@
         <v>3.09120120959282</v>
       </c>
       <c r="E7" t="str">
-        <f t="shared" si="0"/>
+        <f>E6</f>
         <v>3'</v>
       </c>
       <c r="F7">
         <v>9</v>
       </c>
+      <c r="G7"/>
       <c r="T7" s="5"/>
       <c r="U7" s="5"/>
       <c r="V7" s="5"/>
@@ -1363,26 +1367,15 @@
       <c r="AB7" s="5"/>
       <c r="AC7" s="5"/>
     </row>
-    <row r="8" spans="1:29">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8">
-        <v>3205.51260462066</v>
-      </c>
-      <c r="C8">
-        <v>447432.34</v>
-      </c>
-      <c r="D8">
-        <v>3.98962201035817</v>
-      </c>
+    <row r="8" spans="5:29">
       <c r="E8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="E8:E53" si="0">E7</f>
         <v>3'</v>
       </c>
       <c r="F8">
         <v>10</v>
       </c>
+      <c r="G8"/>
       <c r="T8" s="5"/>
       <c r="U8" s="5"/>
       <c r="V8" s="5"/>
@@ -1412,6 +1405,7 @@
       <c r="F9">
         <v>11</v>
       </c>
+      <c r="G9"/>
       <c r="T9" s="5"/>
       <c r="U9" s="5"/>
       <c r="V9" s="5"/>
@@ -1441,6 +1435,7 @@
       <c r="F10">
         <v>12</v>
       </c>
+      <c r="G10"/>
       <c r="T10" s="5"/>
       <c r="U10" s="5"/>
       <c r="V10" s="5"/>
@@ -1985,7 +1980,7 @@
         <v>14.9421974098364</v>
       </c>
       <c r="E36" t="str">
-        <f t="shared" ref="E36:E54" si="1">E35</f>
+        <f t="shared" si="0"/>
         <v>3'</v>
       </c>
       <c r="F36">
@@ -2006,7 +2001,7 @@
         <v>15.0010001019319</v>
       </c>
       <c r="E37" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3'</v>
       </c>
       <c r="F37">
@@ -2027,7 +2022,7 @@
         <v>15.2678781942209</v>
       </c>
       <c r="E38" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3'</v>
       </c>
       <c r="F38">
@@ -2048,7 +2043,7 @@
         <v>15.2678781942209</v>
       </c>
       <c r="E39" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3'</v>
       </c>
       <c r="F39">
@@ -2069,7 +2064,7 @@
         <v>15.3583739514828</v>
       </c>
       <c r="E40" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3'</v>
       </c>
       <c r="F40">
@@ -2090,7 +2085,7 @@
         <v>15.3900409853141</v>
       </c>
       <c r="E41" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3'</v>
       </c>
       <c r="F41">
@@ -2111,7 +2106,7 @@
         <v>15.4488665258567</v>
       </c>
       <c r="E42" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3'</v>
       </c>
       <c r="F42">
@@ -2132,7 +2127,7 @@
         <v>15.5393673594475</v>
       </c>
       <c r="E43" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3'</v>
       </c>
       <c r="F43">
@@ -2153,7 +2148,7 @@
         <v>15.6027141030312</v>
       </c>
       <c r="E44" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3'</v>
       </c>
       <c r="F44">
@@ -2174,7 +2169,7 @@
         <v>15.8108852680206</v>
       </c>
       <c r="E45" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3'</v>
       </c>
       <c r="F45">
@@ -2195,7 +2190,7 @@
         <v>15.7792122260412</v>
       </c>
       <c r="E46" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3'</v>
       </c>
       <c r="F46">
@@ -2216,7 +2211,7 @@
         <v>15.838043818442</v>
       </c>
       <c r="E47" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3'</v>
       </c>
       <c r="F47">
@@ -2237,7 +2232,7 @@
         <v>15.8697345192909</v>
       </c>
       <c r="E48" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3'</v>
       </c>
       <c r="F48">
@@ -2258,7 +2253,7 @@
         <v>15.9285836255232</v>
       </c>
       <c r="E49" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3'</v>
       </c>
       <c r="F49">
@@ -2279,7 +2274,7 @@
         <v>15.9919585183938</v>
       </c>
       <c r="E50" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3'</v>
       </c>
       <c r="F50">
@@ -2300,7 +2295,7 @@
         <v>16.136828825442</v>
       </c>
       <c r="E51" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3'</v>
       </c>
       <c r="F51">
@@ -2321,7 +2316,7 @@
         <v>16.2590953763008</v>
       </c>
       <c r="E52" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3'</v>
       </c>
       <c r="F52">
@@ -2342,7 +2337,7 @@
         <v>16.2002343610605</v>
       </c>
       <c r="E53" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3'</v>
       </c>
       <c r="F53">
@@ -2392,14 +2387,14 @@
         <v>16.4085768834432</v>
       </c>
       <c r="E56" t="str">
-        <f t="shared" ref="E55:E75" si="2">E55</f>
+        <f t="shared" ref="E55:E75" si="1">E55</f>
         <v>3'</v>
       </c>
       <c r="F56">
         <v>58</v>
       </c>
     </row>
-    <row r="57" spans="1:12">
+    <row r="57" spans="1:6">
       <c r="A57" t="s">
         <v>8</v>
       </c>
@@ -2413,18 +2408,14 @@
         <v>16.4085768834432</v>
       </c>
       <c r="E57" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3'</v>
       </c>
       <c r="F57">
         <v>59</v>
       </c>
-      <c r="I57" s="5"/>
-      <c r="J57" s="5"/>
-      <c r="K57" s="5"/>
-      <c r="L57" s="5"/>
-    </row>
-    <row r="58" spans="1:12">
+    </row>
+    <row r="58" spans="1:6">
       <c r="A58" t="s">
         <v>10</v>
       </c>
@@ -2438,18 +2429,14 @@
         <v>16.4402790184498</v>
       </c>
       <c r="E58" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3'</v>
       </c>
       <c r="F58">
         <v>60</v>
       </c>
-      <c r="I58" s="5"/>
-      <c r="J58" s="5"/>
-      <c r="K58" s="5"/>
-      <c r="L58" s="5"/>
-    </row>
-    <row r="59" spans="1:12">
+    </row>
+    <row r="59" spans="1:6">
       <c r="A59" t="s">
         <v>8</v>
       </c>
@@ -2463,18 +2450,14 @@
         <v>16.4719959691842</v>
       </c>
       <c r="E59" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3'</v>
       </c>
       <c r="F59">
         <v>61</v>
       </c>
-      <c r="I59" s="5"/>
-      <c r="J59" s="5"/>
-      <c r="K59" s="5"/>
-      <c r="L59" s="5"/>
-    </row>
-    <row r="60" spans="1:12">
+    </row>
+    <row r="60" spans="1:6">
       <c r="A60" t="s">
         <v>9</v>
       </c>
@@ -2488,16 +2471,12 @@
         <v>16.6532833770593</v>
       </c>
       <c r="E60" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3'</v>
       </c>
       <c r="F60">
         <v>62</v>
       </c>
-      <c r="I60" s="5"/>
-      <c r="J60" s="5"/>
-      <c r="K60" s="5"/>
-      <c r="L60" s="5"/>
     </row>
     <row r="61" spans="1:6">
       <c r="A61" t="s">
@@ -2513,7 +2492,7 @@
         <v>16.6170121685346</v>
       </c>
       <c r="E61" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3'</v>
       </c>
       <c r="F61">
@@ -2534,7 +2513,7 @@
         <v>16.6170121685346</v>
       </c>
       <c r="E62" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3'</v>
       </c>
       <c r="F62">
@@ -2555,7 +2534,7 @@
         <v>16.6532833770593</v>
       </c>
       <c r="E63" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3'</v>
       </c>
       <c r="F63">
@@ -2576,7 +2555,7 @@
         <v>16.6804952756246</v>
       </c>
       <c r="E64" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3'</v>
       </c>
       <c r="F64">
@@ -2597,7 +2576,7 @@
         <v>16.7077064847628</v>
       </c>
       <c r="E65" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3'</v>
       </c>
       <c r="F65">
@@ -2618,7 +2597,7 @@
         <v>16.7394507920424</v>
       </c>
       <c r="E66" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3'</v>
       </c>
       <c r="F66">
@@ -2639,7 +2618,7 @@
         <v>16.7711935019175</v>
       </c>
       <c r="E67" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3'</v>
       </c>
       <c r="F67">
@@ -2660,7 +2639,7 @@
         <v>16.8891516681194</v>
       </c>
       <c r="E68" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3'</v>
       </c>
       <c r="F68">
@@ -2681,7 +2660,7 @@
         <v>16.8619266088486</v>
       </c>
       <c r="E69" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3'</v>
       </c>
       <c r="F69">
@@ -2702,7 +2681,7 @@
         <v>16.8619266088486</v>
       </c>
       <c r="E70" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3'</v>
       </c>
       <c r="F70">
@@ -2723,7 +2702,7 @@
         <v>16.9209141190529</v>
       </c>
       <c r="E71" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3'</v>
       </c>
       <c r="F71">
@@ -2744,7 +2723,7 @@
         <v>16.9209141190529</v>
       </c>
       <c r="E72" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3'</v>
       </c>
       <c r="F72">
@@ -2765,7 +2744,7 @@
         <v>16.9526782091141</v>
       </c>
       <c r="E73" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3'</v>
       </c>
       <c r="F73">
@@ -2786,7 +2765,7 @@
         <v>16.9799155588627</v>
       </c>
       <c r="E74" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3'</v>
       </c>
       <c r="F74">
@@ -2807,7 +2786,7 @@
         <v>17.0707158263207</v>
       </c>
       <c r="E75" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3'</v>
       </c>
       <c r="F75">
@@ -2983,7 +2962,7 @@
         <v>7.47073565281232</v>
       </c>
       <c r="E84" t="str">
-        <f t="shared" ref="E84:E118" si="3">E83</f>
+        <f t="shared" ref="E84:E118" si="2">E83</f>
         <v>5'</v>
       </c>
       <c r="F84">
@@ -3004,7 +2983,7 @@
         <v>8.01259183443387</v>
       </c>
       <c r="E85" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5'</v>
       </c>
       <c r="F85">
@@ -3025,7 +3004,7 @@
         <v>8.60863366084099</v>
       </c>
       <c r="E86" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5'</v>
       </c>
       <c r="F86">
@@ -3046,7 +3025,7 @@
         <v>9.11888837572733</v>
       </c>
       <c r="E87" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5'</v>
       </c>
       <c r="F87">
@@ -3067,7 +3046,7 @@
         <v>9.80984763460159</v>
       </c>
       <c r="E88" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5'</v>
       </c>
       <c r="F88">
@@ -3088,7 +3067,7 @@
         <v>10.4104951595942</v>
       </c>
       <c r="E89" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5'</v>
       </c>
       <c r="F89">
@@ -3109,7 +3088,7 @@
         <v>10.6769516682307</v>
       </c>
       <c r="E90" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5'</v>
       </c>
       <c r="F90">
@@ -3130,7 +3109,7 @@
         <v>10.9795485094865</v>
       </c>
       <c r="E91" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5'</v>
       </c>
       <c r="F91">
@@ -3151,7 +3130,7 @@
         <v>11.2505395348549</v>
       </c>
       <c r="E92" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5'</v>
       </c>
       <c r="F92">
@@ -3172,7 +3151,7 @@
         <v>11.5170138434251</v>
       </c>
       <c r="E93" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5'</v>
       </c>
       <c r="F93">
@@ -3193,7 +3172,7 @@
         <v>11.760917841959</v>
       </c>
       <c r="E94" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5'</v>
       </c>
       <c r="F94">
@@ -3214,7 +3193,7 @@
         <v>12.0319247599125</v>
       </c>
       <c r="E95" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5'</v>
       </c>
       <c r="F95">
@@ -3235,7 +3214,7 @@
         <v>12.388759600687</v>
       </c>
       <c r="E96" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5'</v>
       </c>
       <c r="F96">
@@ -3256,7 +3235,7 @@
         <v>12.5694418763796</v>
       </c>
       <c r="E97" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5'</v>
       </c>
       <c r="F97">
@@ -3277,7 +3256,7 @@
         <v>12.7817702587128</v>
       </c>
       <c r="E98" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5'</v>
       </c>
       <c r="F98">
@@ -3298,7 +3277,7 @@
         <v>12.930852951177</v>
       </c>
       <c r="E99" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5'</v>
       </c>
       <c r="F99">
@@ -3319,7 +3298,7 @@
         <v>13.1431922173182</v>
       </c>
       <c r="E100" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5'</v>
       </c>
       <c r="F100">
@@ -3340,7 +3319,7 @@
         <v>13.2606781518141</v>
       </c>
       <c r="E101" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5'</v>
       </c>
       <c r="F101">
@@ -3361,7 +3340,7 @@
         <v>13.4097915605386</v>
       </c>
       <c r="E102" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5'</v>
       </c>
       <c r="F102">
@@ -3382,7 +3361,7 @@
         <v>13.680911918052</v>
       </c>
       <c r="E103" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5'</v>
       </c>
       <c r="F103">
@@ -3403,7 +3382,7 @@
         <v>13.766782893308</v>
       </c>
       <c r="E104" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5'</v>
       </c>
       <c r="F104">
@@ -3424,7 +3403,7 @@
         <v>13.9204612350146</v>
       </c>
       <c r="E105" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5'</v>
       </c>
       <c r="F105">
@@ -3445,7 +3424,7 @@
         <v>14.0108577267011</v>
       </c>
       <c r="E106" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5'</v>
       </c>
       <c r="F106">
@@ -3466,7 +3445,7 @@
         <v>14.1012540256659</v>
       </c>
       <c r="E107" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5'</v>
       </c>
       <c r="F107">
@@ -3487,7 +3466,7 @@
         <v>14.2187835271835</v>
       </c>
       <c r="E108" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5'</v>
       </c>
       <c r="F108">
@@ -3508,7 +3487,7 @@
         <v>14.3408405200322</v>
       </c>
       <c r="E109" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5'</v>
       </c>
       <c r="F109">
@@ -3529,7 +3508,7 @@
         <v>14.4267348106384</v>
       </c>
       <c r="E110" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5'</v>
       </c>
       <c r="F110">
@@ -3550,7 +3529,7 @@
         <v>14.6075680609226</v>
       </c>
       <c r="E111" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5'</v>
       </c>
       <c r="F111">
@@ -3571,7 +3550,7 @@
         <v>14.6980083262603</v>
       </c>
       <c r="E112" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5'</v>
       </c>
       <c r="F112">
@@ -3592,7 +3571,7 @@
         <v>14.7613065337817</v>
       </c>
       <c r="E113" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5'</v>
       </c>
       <c r="F113">
@@ -3613,7 +3592,7 @@
         <v>14.8517429347515</v>
       </c>
       <c r="E114" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5'</v>
       </c>
       <c r="F114">
@@ -3634,7 +3613,7 @@
         <v>14.9421974098364</v>
       </c>
       <c r="E115" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5'</v>
       </c>
       <c r="F115">
@@ -3655,7 +3634,7 @@
         <v>15.0869539594332</v>
       </c>
       <c r="E116" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5'</v>
       </c>
       <c r="F116">
@@ -3676,7 +3655,7 @@
         <v>15.1231340523243</v>
       </c>
       <c r="E117" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5'</v>
       </c>
       <c r="F117">
@@ -3697,7 +3676,7 @@
         <v>15.2090786671321</v>
       </c>
       <c r="E118" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5'</v>
       </c>
       <c r="F118">
@@ -3706,7 +3685,7 @@
     </row>
     <row r="119" spans="5:6">
       <c r="E119" t="str">
-        <f t="shared" ref="E119:E132" si="4">E118</f>
+        <f t="shared" ref="E119:E132" si="3">E118</f>
         <v>5'</v>
       </c>
       <c r="F119">
@@ -3715,7 +3694,7 @@
     </row>
     <row r="120" spans="5:6">
       <c r="E120" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>5'</v>
       </c>
       <c r="F120">
@@ -3736,7 +3715,7 @@
         <v>15.5122125104745</v>
       </c>
       <c r="E121" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>5'</v>
       </c>
       <c r="F121">
@@ -3757,7 +3736,7 @@
         <v>15.571041792202</v>
       </c>
       <c r="E122" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>5'</v>
       </c>
       <c r="F122">
@@ -3778,7 +3757,7 @@
         <v>15.6027141030312</v>
       </c>
       <c r="E123" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>5'</v>
       </c>
       <c r="F123">
@@ -3799,7 +3778,7 @@
         <v>15.6570179338932</v>
       </c>
       <c r="E124" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>5'</v>
       </c>
       <c r="F124">
@@ -3820,7 +3799,7 @@
         <v>15.7203694855849</v>
       </c>
       <c r="E125" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>5'</v>
       </c>
       <c r="F125">
@@ -3841,7 +3820,7 @@
         <v>15.838043818442</v>
       </c>
       <c r="E126" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>5'</v>
       </c>
       <c r="F126">
@@ -3862,7 +3841,7 @@
         <v>15.838043818442</v>
       </c>
       <c r="E127" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>5'</v>
       </c>
       <c r="F127">
@@ -3924,7 +3903,7 @@
         <v>15.9919585183938</v>
       </c>
       <c r="E130" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>5'</v>
       </c>
       <c r="F130">
@@ -3945,7 +3924,7 @@
         <v>16.050819201835</v>
       </c>
       <c r="E131" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>5'</v>
       </c>
       <c r="F131">
@@ -3966,7 +3945,7 @@
         <v>16.0825053111394</v>
       </c>
       <c r="E132" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>5'</v>
       </c>
       <c r="F132">

</xml_diff>